<commit_message>
Correciones a la conversion a pdf (en proceso)
</commit_message>
<xml_diff>
--- a/Autorizaciones/Autorizacion_TEST-002.xlsx
+++ b/Autorizaciones/Autorizacion_TEST-002.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SSPA Canrig" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -322,7 +322,9 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -333,21 +335,16 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -385,12 +382,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,9 +428,6 @@
     <xf numFmtId="17" fontId="13" fillId="4" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -458,11 +446,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -521,38 +538,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -564,40 +575,31 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -607,7 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -623,19 +624,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -722,7 +729,7 @@
   <oneCellAnchor>
     <from>
       <col>0</col>
-      <colOff>211187</colOff>
+      <colOff>558569</colOff>
       <row>0</row>
       <rowOff>29308</rowOff>
     </from>
@@ -742,7 +749,7 @@
       </blipFill>
       <spPr>
         <a:xfrm>
-          <a:off x="211187" y="29308"/>
+          <a:off x="558569" y="29308"/>
           <a:ext cx="585093" cy="710658"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -751,6 +758,87 @@
         <a:ln>
           <a:prstDash val="solid"/>
         </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>36</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1143000" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>36</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1143000" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>6</col>
+      <colOff>0</colOff>
+      <row>36</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1428750" cy="476250"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1025,651 +1113,1517 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H250"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:H32"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="81" zoomScaleNormal="85" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="10.42578125" customWidth="1" min="2" max="2"/>
-    <col width="15.5703125" customWidth="1" min="3" max="3"/>
-    <col width="17.5703125" customWidth="1" min="4" max="4"/>
-    <col width="11.5703125" customWidth="1" min="5" max="5"/>
-    <col width="10.28515625" customWidth="1" min="6" max="6"/>
-    <col width="20.7109375" customWidth="1" min="7" max="7"/>
-    <col width="12.28515625" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" style="38" min="1" max="1"/>
+    <col width="12.42578125" customWidth="1" style="38" min="2" max="2"/>
+    <col width="19" customWidth="1" style="38" min="3" max="3"/>
+    <col width="17.5703125" customWidth="1" style="38" min="4" max="4"/>
+    <col width="11.5703125" customWidth="1" style="38" min="5" max="5"/>
+    <col width="10.28515625" customWidth="1" style="38" min="6" max="6"/>
+    <col width="26" customWidth="1" style="38" min="7" max="7"/>
+    <col width="12.28515625" customWidth="1" style="38" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="88" t="n"/>
-      <c r="B1" s="89" t="n"/>
-      <c r="C1" s="50" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="38">
+      <c r="A1" s="90" t="n"/>
+      <c r="B1" s="91" t="n"/>
+      <c r="C1" s="57" t="inlineStr">
         <is>
           <t>Autorización de Compra</t>
         </is>
       </c>
-      <c r="D1" s="90" t="n"/>
-      <c r="E1" s="90" t="n"/>
-      <c r="F1" s="90" t="n"/>
-      <c r="G1" s="90" t="n"/>
-      <c r="H1" s="89" t="n"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="91" t="n"/>
-      <c r="B2" s="92" t="n"/>
-      <c r="C2" s="91" t="n"/>
-      <c r="H2" s="92" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="91" t="n"/>
-      <c r="B3" s="92" t="n"/>
-      <c r="C3" s="93" t="n"/>
-      <c r="D3" s="94" t="n"/>
-      <c r="E3" s="94" t="n"/>
-      <c r="F3" s="94" t="n"/>
-      <c r="G3" s="94" t="n"/>
-      <c r="H3" s="95" t="n"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="93" t="n"/>
-      <c r="B4" s="95" t="n"/>
-      <c r="C4" s="34" t="inlineStr">
+      <c r="D1" s="92" t="n"/>
+      <c r="E1" s="92" t="n"/>
+      <c r="F1" s="92" t="n"/>
+      <c r="G1" s="92" t="n"/>
+      <c r="H1" s="91" t="n"/>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="38">
+      <c r="A2" s="93" t="n"/>
+      <c r="B2" s="94" t="n"/>
+      <c r="C2" s="93" t="n"/>
+      <c r="H2" s="94" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="38">
+      <c r="A3" s="93" t="n"/>
+      <c r="B3" s="94" t="n"/>
+      <c r="C3" s="95" t="n"/>
+      <c r="D3" s="39" t="n"/>
+      <c r="E3" s="39" t="n"/>
+      <c r="F3" s="39" t="n"/>
+      <c r="G3" s="39" t="n"/>
+      <c r="H3" s="96" t="n"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1" s="38">
+      <c r="A4" s="95" t="n"/>
+      <c r="B4" s="96" t="n"/>
+      <c r="C4" s="37" t="inlineStr">
         <is>
           <t>Código</t>
         </is>
       </c>
-      <c r="D4" s="32" t="inlineStr">
+      <c r="D4" s="29" t="inlineStr">
         <is>
           <t>FOR-COM-002</t>
         </is>
       </c>
-      <c r="E4" s="32" t="inlineStr">
+      <c r="E4" s="29" t="inlineStr">
         <is>
           <t>Fecha</t>
         </is>
       </c>
-      <c r="F4" s="33" t="n">
+      <c r="F4" s="30" t="n">
         <v>45505</v>
       </c>
-      <c r="G4" s="32" t="inlineStr">
+      <c r="G4" s="29" t="inlineStr">
         <is>
           <t>Revisión</t>
         </is>
       </c>
-      <c r="H4" s="31" t="inlineStr">
+      <c r="H4" s="28" t="inlineStr">
         <is>
           <t>01</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="7.9" customHeight="1">
-      <c r="A5" s="62" t="n"/>
-      <c r="B5" s="62" t="n"/>
-      <c r="C5" s="28" t="n"/>
-      <c r="D5" s="30" t="n"/>
-      <c r="E5" s="28" t="n"/>
-      <c r="F5" s="29" t="n"/>
-      <c r="G5" s="28" t="n"/>
-      <c r="H5" s="27" t="n"/>
+    <row r="5" ht="7.9" customHeight="1" s="38">
+      <c r="A5" s="71" t="n"/>
+      <c r="B5" s="71" t="n"/>
+      <c r="C5" s="25" t="n"/>
+      <c r="D5" s="27" t="n"/>
+      <c r="E5" s="25" t="n"/>
+      <c r="F5" s="26" t="n"/>
+      <c r="G5" s="25" t="n"/>
+      <c r="H5" s="24" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="62" t="n"/>
-      <c r="B6" s="62" t="n"/>
-      <c r="C6" s="62" t="n"/>
-      <c r="D6" s="62" t="n"/>
-      <c r="E6" s="62" t="n"/>
-      <c r="F6" s="51" t="inlineStr">
+      <c r="A6" s="71" t="n"/>
+      <c r="B6" s="71" t="n"/>
+      <c r="C6" s="71" t="n"/>
+      <c r="D6" s="71" t="n"/>
+      <c r="E6" s="71" t="n"/>
+      <c r="F6" s="58" t="inlineStr">
         <is>
           <t>Autorización No.:</t>
         </is>
       </c>
-      <c r="H6" s="96" t="inlineStr">
+      <c r="H6" s="97" t="inlineStr">
         <is>
           <t>TEST-002</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="6.95" customHeight="1">
-      <c r="A7" s="62" t="n"/>
-      <c r="B7" s="62" t="n"/>
-      <c r="C7" s="62" t="n"/>
-      <c r="D7" s="62" t="n"/>
-      <c r="E7" s="62" t="n"/>
-      <c r="F7" s="25" t="n"/>
-      <c r="G7" s="62" t="n"/>
-      <c r="H7" s="62" t="n"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="52" t="inlineStr">
+    <row r="7" ht="6.95" customHeight="1" s="38">
+      <c r="A7" s="71" t="n"/>
+      <c r="B7" s="71" t="n"/>
+      <c r="C7" s="71" t="n"/>
+      <c r="D7" s="71" t="n"/>
+      <c r="E7" s="71" t="n"/>
+      <c r="F7" s="22" t="n"/>
+      <c r="G7" s="71" t="n"/>
+      <c r="H7" s="71" t="n"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" s="38">
+      <c r="A8" s="59" t="inlineStr">
         <is>
           <t xml:space="preserve">Tipo de Solicitud </t>
         </is>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="52" t="n"/>
-      <c r="B9" s="52" t="n"/>
-      <c r="C9" s="52" t="n"/>
-      <c r="D9" s="52" t="n"/>
-      <c r="E9" s="52" t="n"/>
-      <c r="F9" s="52" t="n"/>
-      <c r="H9" s="36" t="n"/>
-    </row>
-    <row r="10" ht="16.5" customHeight="1">
-      <c r="A10" s="37" t="inlineStr">
+    <row r="9" ht="14.25" customHeight="1" s="38">
+      <c r="A9" s="59" t="n"/>
+      <c r="B9" s="59" t="n"/>
+      <c r="C9" s="59" t="n"/>
+      <c r="D9" s="59" t="n"/>
+      <c r="E9" s="59" t="n"/>
+      <c r="F9" s="59" t="n"/>
+      <c r="H9" s="32" t="n"/>
+    </row>
+    <row r="10" ht="16.5" customHeight="1" s="38">
+      <c r="A10" s="33" t="inlineStr">
         <is>
           <t>Maquinaria</t>
         </is>
       </c>
-      <c r="B10" s="22" t="inlineStr"/>
-      <c r="C10" s="38" t="inlineStr">
+      <c r="B10" s="98" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="C10" s="34" t="inlineStr">
         <is>
           <t>Equipo y/o  Htas.</t>
         </is>
       </c>
-      <c r="D10" s="40" t="inlineStr"/>
-      <c r="E10" s="37" t="inlineStr">
+      <c r="D10" s="36" t="inlineStr"/>
+      <c r="E10" s="33" t="inlineStr">
         <is>
           <t xml:space="preserve">Servicios </t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" s="39" t="inlineStr">
+      <c r="G10" s="35" t="inlineStr">
         <is>
           <t>Otros</t>
         </is>
       </c>
-      <c r="H10" s="97" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="6.95" customHeight="1"/>
-    <row r="12" ht="20.1" customHeight="1">
-      <c r="A12" s="35" t="inlineStr">
+      <c r="H10" s="19" t="inlineStr"/>
+    </row>
+    <row r="11" ht="6.95" customHeight="1" s="38"/>
+    <row r="12" ht="20.1" customHeight="1" s="38">
+      <c r="A12" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Solicitante: </t>
         </is>
       </c>
-      <c r="B12" s="53" t="inlineStr">
-        <is>
-          <t>Paola Cortazar</t>
-        </is>
-      </c>
-      <c r="C12" s="94" t="n"/>
-      <c r="D12" s="94" t="n"/>
+      <c r="B12" s="60" t="inlineStr">
+        <is>
+          <t>Alejandro Silvan</t>
+        </is>
+      </c>
+      <c r="C12" s="39" t="n"/>
+      <c r="D12" s="39" t="n"/>
       <c r="E12" s="1" t="n"/>
-      <c r="F12" s="21" t="inlineStr">
+      <c r="F12" s="18" t="inlineStr">
         <is>
           <t>Fecha de solicitud:</t>
         </is>
       </c>
-      <c r="G12" s="98" t="inlineStr">
-        <is>
-          <t>2025/04/04</t>
-        </is>
-      </c>
-      <c r="H12" s="94" t="n"/>
-    </row>
-    <row r="13" ht="24.75" customHeight="1">
-      <c r="A13" s="35" t="inlineStr">
+      <c r="G12" s="99" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="H12" s="39" t="n"/>
+    </row>
+    <row r="13" ht="24.75" customHeight="1" s="38">
+      <c r="A13" s="31" t="inlineStr">
         <is>
           <t>Puesto:</t>
         </is>
       </c>
-      <c r="B13" s="63" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="C13" s="99" t="n"/>
-      <c r="D13" s="99" t="n"/>
+      <c r="B13" s="73" t="inlineStr">
+        <is>
+          <t>Auxiliar Tecnico Administrativo</t>
+        </is>
+      </c>
+      <c r="C13" s="100" t="n"/>
+      <c r="D13" s="100" t="n"/>
       <c r="E13" s="1" t="n"/>
-      <c r="F13" s="21" t="inlineStr">
+      <c r="F13" s="18" t="inlineStr">
         <is>
           <t>Fecha requerida:</t>
         </is>
       </c>
-      <c r="G13" s="98" t="inlineStr">
-        <is>
-          <t>2025/04/04</t>
-        </is>
-      </c>
-      <c r="H13" s="94" t="n"/>
-    </row>
-    <row r="14" ht="20.1" customHeight="1">
-      <c r="A14" s="35" t="inlineStr">
+      <c r="G13" s="99" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="H13" s="39" t="n"/>
+    </row>
+    <row r="14" ht="20.1" customHeight="1" s="38">
+      <c r="A14" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">Área: </t>
         </is>
       </c>
-      <c r="B14" s="63" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="C14" s="99" t="n"/>
-      <c r="D14" s="99" t="n"/>
-      <c r="E14" s="64" t="inlineStr">
+      <c r="B14" s="73" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C14" s="100" t="n"/>
+      <c r="D14" s="100" t="n"/>
+      <c r="E14" s="74" t="inlineStr">
         <is>
           <t>Proyecto y/o Contrato:</t>
         </is>
       </c>
-      <c r="G14" s="100" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="H14" s="99" t="n"/>
-    </row>
-    <row r="15" ht="19.5" customHeight="1">
-      <c r="D15" s="62" t="n"/>
-      <c r="G15" s="20" t="n"/>
-      <c r="H15" s="20" t="n"/>
+      <c r="G14" s="101" t="inlineStr">
+        <is>
+          <t>641003609 / 643024615</t>
+        </is>
+      </c>
+      <c r="H14" s="100" t="n"/>
+    </row>
+    <row r="15" ht="19.5" customHeight="1" s="38">
+      <c r="D15" s="71" t="n"/>
+      <c r="G15" s="17" t="n"/>
+      <c r="H15" s="17" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="61" t="inlineStr">
+      <c r="A16" s="68" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="B16" s="61" t="inlineStr">
+      <c r="B16" s="68" t="inlineStr">
         <is>
           <t>Cantidad</t>
         </is>
       </c>
-      <c r="C16" s="61" t="inlineStr">
+      <c r="C16" s="68" t="inlineStr">
         <is>
           <t xml:space="preserve">Unidad </t>
         </is>
       </c>
-      <c r="D16" s="61" t="inlineStr">
+      <c r="D16" s="68" t="inlineStr">
         <is>
           <t>Descripción</t>
         </is>
       </c>
-      <c r="E16" s="99" t="n"/>
-      <c r="F16" s="101" t="n"/>
-      <c r="G16" s="61" t="inlineStr">
+      <c r="E16" s="100" t="n"/>
+      <c r="F16" s="102" t="n"/>
+      <c r="G16" s="68" t="inlineStr">
         <is>
           <t>Observaciones</t>
         </is>
       </c>
-      <c r="H16" s="101" t="n"/>
-    </row>
-    <row r="17" ht="24.75" customHeight="1">
-      <c r="A17" s="10" t="n">
+      <c r="H16" s="102" t="n"/>
+    </row>
+    <row r="17" ht="24.75" customHeight="1" s="38">
+      <c r="A17" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="9" t="inlineStr">
+      <c r="B17" s="8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C17" s="8" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="D17" s="14" t="inlineStr">
-        <is>
-          <t>TEST 002</t>
-        </is>
-      </c>
-      <c r="E17" s="99" t="n"/>
-      <c r="F17" s="101" t="n"/>
-      <c r="G17" s="14" t="inlineStr">
-        <is>
-          <t>TEST 002</t>
-        </is>
-      </c>
-      <c r="H17" s="101" t="n"/>
-    </row>
-    <row r="18" ht="23.25" customHeight="1">
-      <c r="A18" s="10" t="n">
+      <c r="C17" s="7" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D17" s="13" t="inlineStr">
+        <is>
+          <t>Prueba completa con las tablas truncadas.</t>
+        </is>
+      </c>
+      <c r="E17" s="100" t="n"/>
+      <c r="F17" s="102" t="n"/>
+      <c r="G17" s="103" t="inlineStr">
+        <is>
+          <t>Se prueba desde cero el sistema para correccion de calculos necesarios</t>
+        </is>
+      </c>
+      <c r="H17" s="102" t="n"/>
+    </row>
+    <row r="18" ht="23.25" customHeight="1" s="38">
+      <c r="A18" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="9" t="n"/>
-      <c r="C18" s="8" t="n"/>
-      <c r="D18" s="102" t="n"/>
-      <c r="E18" s="99" t="n"/>
-      <c r="F18" s="101" t="n"/>
-      <c r="G18" s="102" t="n"/>
-      <c r="H18" s="101" t="n"/>
-    </row>
-    <row r="19" ht="25.5" customHeight="1">
-      <c r="A19" s="10" t="n">
+      <c r="B18" s="8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C18" s="7" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D18" s="13" t="inlineStr">
+        <is>
+          <t>Prueba completa del sistema</t>
+        </is>
+      </c>
+      <c r="E18" s="100" t="n"/>
+      <c r="F18" s="102" t="n"/>
+      <c r="G18" s="13" t="inlineStr">
+        <is>
+          <t>Prueba de todo el sistema para calculos del reporte</t>
+        </is>
+      </c>
+      <c r="H18" s="102" t="n"/>
+    </row>
+    <row r="19" ht="25.5" customHeight="1" s="38">
+      <c r="A19" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="18" t="n"/>
-      <c r="C19" s="18" t="n"/>
-      <c r="D19" s="102" t="n"/>
-      <c r="E19" s="99" t="n"/>
-      <c r="F19" s="101" t="n"/>
-      <c r="G19" s="102" t="n"/>
-      <c r="H19" s="101" t="n"/>
-    </row>
-    <row r="20" ht="25.5" customHeight="1">
-      <c r="A20" s="10" t="n">
+      <c r="B19" s="15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C19" s="15" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="D19" s="13" t="inlineStr">
+        <is>
+          <t>Segundo Producto para la segunda prueba</t>
+        </is>
+      </c>
+      <c r="E19" s="100" t="n"/>
+      <c r="F19" s="102" t="n"/>
+      <c r="G19" s="13" t="inlineStr">
+        <is>
+          <t>Se prueba el sistema con multiples productos</t>
+        </is>
+      </c>
+      <c r="H19" s="102" t="n"/>
+    </row>
+    <row r="20" ht="25.5" customHeight="1" s="38">
+      <c r="A20" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="18" t="n"/>
-      <c r="C20" s="18" t="n"/>
-      <c r="D20" s="102" t="n"/>
-      <c r="E20" s="99" t="n"/>
-      <c r="F20" s="101" t="n"/>
-      <c r="G20" s="102" t="n"/>
-      <c r="H20" s="101" t="n"/>
-    </row>
-    <row r="21" ht="24" customHeight="1">
-      <c r="A21" s="10" t="n">
+      <c r="B20" s="15" t="n"/>
+      <c r="C20" s="15" t="n"/>
+      <c r="D20" s="104" t="n"/>
+      <c r="E20" s="100" t="n"/>
+      <c r="F20" s="102" t="n"/>
+      <c r="G20" s="105" t="n"/>
+      <c r="H20" s="102" t="n"/>
+    </row>
+    <row r="21" ht="24" customHeight="1" s="38">
+      <c r="A21" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="15" t="n"/>
-      <c r="C21" s="15" t="n"/>
-      <c r="D21" s="102" t="n"/>
-      <c r="E21" s="99" t="n"/>
-      <c r="F21" s="101" t="n"/>
-      <c r="G21" s="102" t="n"/>
-      <c r="H21" s="101" t="n"/>
-    </row>
-    <row r="22" ht="25.5" customHeight="1">
-      <c r="A22" s="10" t="n">
+      <c r="B21" s="14" t="n"/>
+      <c r="C21" s="14" t="n"/>
+      <c r="D21" s="104" t="n"/>
+      <c r="E21" s="100" t="n"/>
+      <c r="F21" s="102" t="n"/>
+      <c r="G21" s="105" t="n"/>
+      <c r="H21" s="102" t="n"/>
+    </row>
+    <row r="22" ht="25.5" customHeight="1" s="38">
+      <c r="A22" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="15" t="n"/>
-      <c r="C22" s="15" t="n"/>
-      <c r="D22" s="102" t="n"/>
-      <c r="E22" s="99" t="n"/>
-      <c r="F22" s="101" t="n"/>
-      <c r="G22" s="102" t="n"/>
-      <c r="H22" s="101" t="n"/>
-    </row>
-    <row r="23" ht="23.25" customHeight="1">
-      <c r="A23" s="10" t="n">
+      <c r="B22" s="14" t="n"/>
+      <c r="C22" s="14" t="n"/>
+      <c r="D22" s="104" t="n"/>
+      <c r="E22" s="100" t="n"/>
+      <c r="F22" s="102" t="n"/>
+      <c r="G22" s="105" t="n"/>
+      <c r="H22" s="102" t="n"/>
+    </row>
+    <row r="23" ht="23.25" customHeight="1" s="38">
+      <c r="A23" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="15" t="n"/>
-      <c r="C23" s="15" t="n"/>
-      <c r="D23" s="102" t="n"/>
-      <c r="E23" s="99" t="n"/>
-      <c r="F23" s="101" t="n"/>
-      <c r="G23" s="102" t="n"/>
-      <c r="H23" s="101" t="n"/>
-    </row>
-    <row r="24" ht="23.25" customHeight="1">
-      <c r="A24" s="10" t="n">
+      <c r="B23" s="14" t="n"/>
+      <c r="C23" s="14" t="n"/>
+      <c r="D23" s="104" t="n"/>
+      <c r="E23" s="100" t="n"/>
+      <c r="F23" s="102" t="n"/>
+      <c r="G23" s="105" t="n"/>
+      <c r="H23" s="102" t="n"/>
+    </row>
+    <row r="24" ht="23.25" customHeight="1" s="38">
+      <c r="A24" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="15" t="n"/>
-      <c r="C24" s="15" t="n"/>
-      <c r="D24" s="102" t="n"/>
-      <c r="E24" s="99" t="n"/>
-      <c r="F24" s="101" t="n"/>
-      <c r="G24" s="54" t="n"/>
-      <c r="H24" s="56" t="n"/>
-    </row>
-    <row r="25" ht="23.25" customHeight="1">
-      <c r="A25" s="10" t="n">
+      <c r="B24" s="14" t="n"/>
+      <c r="C24" s="14" t="n"/>
+      <c r="D24" s="104" t="n"/>
+      <c r="E24" s="100" t="n"/>
+      <c r="F24" s="102" t="n"/>
+      <c r="G24" s="105" t="n"/>
+      <c r="H24" s="102" t="n"/>
+    </row>
+    <row r="25" ht="23.25" customHeight="1" s="38">
+      <c r="A25" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="15" t="n"/>
-      <c r="C25" s="15" t="n"/>
-      <c r="D25" s="102" t="n"/>
-      <c r="E25" s="99" t="n"/>
-      <c r="F25" s="101" t="n"/>
-      <c r="G25" s="54" t="n"/>
-      <c r="H25" s="56" t="n"/>
-    </row>
-    <row r="26" ht="21" customHeight="1">
-      <c r="A26" s="10" t="n">
+      <c r="B25" s="14" t="n"/>
+      <c r="C25" s="14" t="n"/>
+      <c r="D25" s="104" t="n"/>
+      <c r="E25" s="100" t="n"/>
+      <c r="F25" s="102" t="n"/>
+      <c r="G25" s="105" t="n"/>
+      <c r="H25" s="102" t="n"/>
+    </row>
+    <row r="26" ht="21" customHeight="1" s="38">
+      <c r="A26" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="15" t="n"/>
-      <c r="C26" s="15" t="n"/>
-      <c r="D26" s="102" t="n"/>
-      <c r="E26" s="99" t="n"/>
-      <c r="F26" s="101" t="n"/>
-      <c r="G26" s="102" t="n"/>
-      <c r="H26" s="101" t="n"/>
-    </row>
-    <row r="27" hidden="1" ht="26.25" customHeight="1">
-      <c r="A27" s="10" t="n">
+      <c r="B26" s="14" t="n"/>
+      <c r="C26" s="14" t="n"/>
+      <c r="D26" s="104" t="n"/>
+      <c r="E26" s="100" t="n"/>
+      <c r="F26" s="102" t="n"/>
+      <c r="G26" s="105" t="n"/>
+      <c r="H26" s="102" t="n"/>
+    </row>
+    <row r="27" hidden="1" ht="26.25" customHeight="1" s="38">
+      <c r="A27" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="B27" s="14" t="n"/>
-      <c r="C27" s="13" t="n"/>
-      <c r="D27" s="102" t="n"/>
-      <c r="E27" s="99" t="n"/>
-      <c r="F27" s="101" t="n"/>
-      <c r="G27" s="102" t="n"/>
-      <c r="H27" s="101" t="n"/>
-    </row>
-    <row r="28" hidden="1" ht="26.25" customHeight="1">
-      <c r="A28" s="10" t="n">
+      <c r="B27" s="13" t="n"/>
+      <c r="C27" s="12" t="n"/>
+      <c r="D27" s="104" t="n"/>
+      <c r="E27" s="100" t="n"/>
+      <c r="F27" s="102" t="n"/>
+      <c r="G27" s="104" t="n"/>
+      <c r="H27" s="102" t="n"/>
+    </row>
+    <row r="28" hidden="1" ht="26.25" customHeight="1" s="38">
+      <c r="A28" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="B28" s="14" t="n"/>
-      <c r="C28" s="13" t="n"/>
-      <c r="D28" s="102" t="n"/>
-      <c r="E28" s="99" t="n"/>
-      <c r="F28" s="101" t="n"/>
-      <c r="G28" s="12" t="n"/>
-      <c r="H28" s="11" t="n"/>
-    </row>
-    <row r="29" hidden="1" ht="8.449999999999999" customHeight="1">
-      <c r="A29" s="10" t="n">
+      <c r="B28" s="13" t="n"/>
+      <c r="C28" s="12" t="n"/>
+      <c r="D28" s="104" t="n"/>
+      <c r="E28" s="100" t="n"/>
+      <c r="F28" s="102" t="n"/>
+      <c r="G28" s="11" t="n"/>
+      <c r="H28" s="10" t="n"/>
+    </row>
+    <row r="29" hidden="1" ht="8.449999999999999" customHeight="1" s="38">
+      <c r="A29" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="B29" s="9" t="n"/>
-      <c r="C29" s="8" t="n"/>
-      <c r="D29" s="103" t="n"/>
-      <c r="E29" s="99" t="n"/>
-      <c r="F29" s="101" t="n"/>
-      <c r="G29" s="102" t="n"/>
-      <c r="H29" s="101" t="n"/>
-    </row>
-    <row r="30" ht="30.75" customHeight="1">
-      <c r="A30" s="86" t="inlineStr">
+      <c r="B29" s="8" t="n"/>
+      <c r="C29" s="7" t="n"/>
+      <c r="D29" s="106" t="n"/>
+      <c r="E29" s="100" t="n"/>
+      <c r="F29" s="102" t="n"/>
+      <c r="G29" s="104" t="n"/>
+      <c r="H29" s="102" t="n"/>
+    </row>
+    <row r="30" ht="19.5" customHeight="1" s="38">
+      <c r="A30" s="44" t="inlineStr">
         <is>
           <t>Observaciones:</t>
         </is>
       </c>
-      <c r="B30" s="104" t="inlineStr">
+      <c r="B30" s="107" t="inlineStr">
         <is>
           <t>Tarjeta de Débito</t>
         </is>
       </c>
-      <c r="C30" s="90" t="n"/>
-      <c r="D30" s="90" t="n"/>
-      <c r="E30" s="90" t="n"/>
-      <c r="F30" s="90" t="n"/>
-      <c r="G30" s="90" t="n"/>
-      <c r="H30" s="89" t="n"/>
-    </row>
-    <row r="31" ht="15" customHeight="1">
-      <c r="A31" s="76" t="inlineStr">
+      <c r="C30" s="92" t="n"/>
+      <c r="D30" s="92" t="n"/>
+      <c r="E30" s="92" t="n"/>
+      <c r="F30" s="92" t="n"/>
+      <c r="G30" s="92" t="n"/>
+      <c r="H30" s="91" t="n"/>
+    </row>
+    <row r="31" ht="15.75" customHeight="1" s="38">
+      <c r="A31" s="43" t="inlineStr">
         <is>
           <t>Proveedor:</t>
         </is>
       </c>
-      <c r="B31" s="105" t="inlineStr">
-        <is>
-          <t>44 - GUSTAVO ESTRADA AGUILAR</t>
-        </is>
-      </c>
-      <c r="H31" s="92" t="n"/>
+      <c r="B31" s="108" t="inlineStr">
+        <is>
+          <t>6 - CESAR REYES IZQUIERDO</t>
+        </is>
+      </c>
+      <c r="H31" s="94" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="66" t="inlineStr">
+      <c r="A32" s="42" t="inlineStr">
         <is>
           <t>Monto:</t>
         </is>
       </c>
-      <c r="B32" s="106" t="inlineStr">
-        <is>
-          <t>10000</t>
-        </is>
-      </c>
-      <c r="C32" s="94" t="n"/>
-      <c r="D32" s="94" t="n"/>
-      <c r="E32" s="94" t="n"/>
-      <c r="F32" s="94" t="n"/>
-      <c r="G32" s="94" t="n"/>
-      <c r="H32" s="95" t="n"/>
-    </row>
-    <row r="33" ht="12" customHeight="1">
-      <c r="A33" s="69" t="inlineStr">
+      <c r="B32" s="109" t="inlineStr">
+        <is>
+          <t>58000</t>
+        </is>
+      </c>
+      <c r="C32" s="39" t="n"/>
+      <c r="D32" s="39" t="n"/>
+      <c r="E32" s="39" t="n"/>
+      <c r="F32" s="39" t="n"/>
+      <c r="G32" s="39" t="n"/>
+      <c r="H32" s="96" t="n"/>
+    </row>
+    <row r="33" ht="28.5" customHeight="1" s="38">
+      <c r="A33" s="48" t="inlineStr">
         <is>
           <t>NOTA: Cuando el producto, equipo y/o servicio sea especializado deberá anexarse su ficha técnica, cuando asi aplique, y sus requerimientos de manera específica y precisa.</t>
         </is>
       </c>
-    </row>
-    <row r="34" ht="12" customHeight="1"/>
-    <row r="35">
-      <c r="A35" s="7" t="n"/>
-      <c r="B35" s="7" t="n"/>
-      <c r="C35" s="7" t="n"/>
-      <c r="D35" s="7" t="n"/>
-      <c r="E35" s="7" t="n"/>
-      <c r="F35" s="7" t="n"/>
-      <c r="G35" s="7" t="n"/>
-      <c r="H35" s="7" t="n"/>
-    </row>
-    <row r="36" ht="30" customHeight="1">
-      <c r="A36" s="70" t="inlineStr">
+      <c r="B33" s="92" t="n"/>
+      <c r="C33" s="92" t="n"/>
+      <c r="D33" s="92" t="n"/>
+      <c r="E33" s="92" t="n"/>
+      <c r="F33" s="92" t="n"/>
+      <c r="G33" s="92" t="n"/>
+      <c r="H33" s="92" t="n"/>
+    </row>
+    <row r="34" ht="12" customHeight="1" s="38">
+      <c r="A34" s="41" t="n"/>
+      <c r="B34" s="41" t="n"/>
+      <c r="C34" s="41" t="n"/>
+      <c r="D34" s="41" t="n"/>
+      <c r="E34" s="41" t="n"/>
+      <c r="F34" s="41" t="n"/>
+      <c r="G34" s="41" t="n"/>
+      <c r="H34" s="41" t="n"/>
+    </row>
+    <row r="35" ht="27" customHeight="1" s="38">
+      <c r="A35" s="6" t="n"/>
+      <c r="B35" s="6" t="n"/>
+      <c r="C35" s="6" t="n"/>
+      <c r="D35" s="6" t="n"/>
+      <c r="E35" s="6" t="n"/>
+      <c r="F35" s="6" t="n"/>
+      <c r="G35" s="6" t="n"/>
+      <c r="H35" s="6" t="n"/>
+    </row>
+    <row r="36" ht="30" customHeight="1" s="38">
+      <c r="A36" s="49" t="inlineStr">
         <is>
           <t xml:space="preserve">Solicita </t>
         </is>
       </c>
-      <c r="D36" s="6" t="n"/>
-      <c r="E36" s="6" t="n"/>
-      <c r="G36" s="70" t="inlineStr">
+      <c r="D36" s="5" t="n"/>
+      <c r="E36" s="5" t="n"/>
+      <c r="G36" s="49" t="inlineStr">
         <is>
           <t>Autoriza</t>
         </is>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1">
-      <c r="A37" s="5" t="n"/>
-      <c r="B37" s="5" t="n"/>
-      <c r="C37" s="5" t="n"/>
-      <c r="D37" s="4" t="n"/>
-      <c r="E37" s="4" t="n"/>
-      <c r="G37" s="72" t="n"/>
-    </row>
-    <row r="38" ht="18.75" customHeight="1">
-      <c r="D38" s="3" t="n"/>
-      <c r="E38" s="3" t="n"/>
-      <c r="F38" s="3" t="n"/>
-      <c r="G38" s="94" t="n"/>
-      <c r="H38" s="94" t="n"/>
-    </row>
-    <row r="39" ht="15" customHeight="1">
-      <c r="A39" s="81" t="inlineStr">
+    <row r="37" ht="15" customHeight="1" s="38">
+      <c r="A37" s="4" t="n"/>
+      <c r="B37" s="4" t="n"/>
+      <c r="C37" s="4" t="n"/>
+      <c r="D37" s="3" t="n"/>
+      <c r="E37" s="3" t="n"/>
+    </row>
+    <row r="38" ht="18.75" customHeight="1" s="38">
+      <c r="D38" s="2" t="n"/>
+      <c r="E38" s="2" t="n"/>
+      <c r="F38" s="2" t="n"/>
+      <c r="H38" s="39" t="n"/>
+    </row>
+    <row r="39" ht="15" customHeight="1" s="38">
+      <c r="A39" s="47" t="inlineStr">
         <is>
           <t xml:space="preserve">Nombre: </t>
         </is>
       </c>
-      <c r="B39" s="107" t="inlineStr">
-        <is>
-          <t>Paola Cortazar</t>
-        </is>
-      </c>
-      <c r="C39" s="90" t="n"/>
+      <c r="B39" s="110" t="inlineStr">
+        <is>
+          <t>Alejandro Silvan</t>
+        </is>
+      </c>
+      <c r="C39" s="92" t="n"/>
       <c r="D39" s="1" t="n"/>
-      <c r="G39" s="65" t="inlineStr">
+      <c r="G39" s="77" t="inlineStr">
         <is>
           <t>Nombre: Dalia Guzmán Palomino</t>
         </is>
       </c>
-      <c r="H39" s="90" t="n"/>
-    </row>
-    <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="82" t="inlineStr">
+      <c r="H39" s="92" t="n"/>
+    </row>
+    <row r="40" ht="12.75" customHeight="1" s="38">
+      <c r="A40" s="46" t="inlineStr">
         <is>
           <t>Puesto:</t>
         </is>
       </c>
-      <c r="B40" s="78" t="inlineStr">
-        <is>
-          <t>TEST</t>
+      <c r="B40" s="40" t="inlineStr">
+        <is>
+          <t>Auxiliar Tecnico Administrativo</t>
         </is>
       </c>
       <c r="D40" s="1" t="n"/>
-      <c r="G40" s="78" t="inlineStr">
+      <c r="G40" s="40" t="inlineStr">
         <is>
           <t xml:space="preserve">Puesto: Gerente General </t>
         </is>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="n"/>
-      <c r="B41" s="2" t="n"/>
-      <c r="C41" s="2" t="n"/>
-      <c r="D41" s="1" t="n"/>
-      <c r="F41" s="1" t="n"/>
-      <c r="G41" s="1" t="n"/>
-    </row>
-    <row r="42">
-      <c r="D42" s="71" t="n"/>
-      <c r="F42" s="1" t="n"/>
+      <c r="H40" s="40" t="n"/>
+    </row>
+    <row r="41" ht="17.25" customHeight="1" s="38"/>
+    <row r="43">
+      <c r="B43" s="45" t="n"/>
+      <c r="C43" s="45" t="n"/>
+    </row>
+    <row r="44">
+      <c r="B44" s="45" t="n"/>
+      <c r="C44" s="45" t="n"/>
+    </row>
+    <row r="45">
+      <c r="B45" s="45" t="n"/>
+      <c r="C45" s="45" t="n"/>
+    </row>
+    <row r="46">
+      <c r="B46" s="45" t="n"/>
+      <c r="C46" s="45" t="n"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="45" t="n"/>
+      <c r="C47" s="45" t="n"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="45" t="n"/>
+      <c r="C48" s="45" t="n"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="45" t="n"/>
+      <c r="C49" s="45" t="n"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="45" t="n"/>
+      <c r="C50" s="45" t="n"/>
+    </row>
+    <row r="51">
+      <c r="B51" s="45" t="n"/>
+      <c r="C51" s="45" t="n"/>
+    </row>
+    <row r="52">
+      <c r="B52" s="45" t="n"/>
+      <c r="C52" s="45" t="n"/>
+    </row>
+    <row r="53">
+      <c r="B53" s="45" t="n"/>
+      <c r="C53" s="45" t="n"/>
+    </row>
+    <row r="54">
+      <c r="B54" s="45" t="n"/>
+      <c r="C54" s="45" t="n"/>
+    </row>
+    <row r="55">
+      <c r="B55" s="45" t="n"/>
+      <c r="C55" s="45" t="n"/>
+    </row>
+    <row r="56">
+      <c r="B56" s="45" t="n"/>
+      <c r="C56" s="45" t="n"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="45" t="n"/>
+      <c r="C57" s="45" t="n"/>
+    </row>
+    <row r="58">
+      <c r="B58" s="45" t="n"/>
+      <c r="C58" s="45" t="n"/>
+    </row>
+    <row r="59">
+      <c r="B59" s="45" t="n"/>
+      <c r="C59" s="45" t="n"/>
+    </row>
+    <row r="60">
+      <c r="B60" s="45" t="n"/>
+      <c r="C60" s="45" t="n"/>
+    </row>
+    <row r="61">
+      <c r="B61" s="45" t="n"/>
+      <c r="C61" s="45" t="n"/>
+    </row>
+    <row r="62">
+      <c r="B62" s="45" t="n"/>
+      <c r="C62" s="45" t="n"/>
+    </row>
+    <row r="63">
+      <c r="B63" s="45" t="n"/>
+      <c r="C63" s="45" t="n"/>
+    </row>
+    <row r="64">
+      <c r="B64" s="45" t="n"/>
+      <c r="C64" s="45" t="n"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="45" t="n"/>
+      <c r="C65" s="45" t="n"/>
+    </row>
+    <row r="66">
+      <c r="B66" s="45" t="n"/>
+      <c r="C66" s="45" t="n"/>
+    </row>
+    <row r="67">
+      <c r="B67" s="45" t="n"/>
+      <c r="C67" s="45" t="n"/>
+    </row>
+    <row r="68">
+      <c r="B68" s="45" t="n"/>
+      <c r="C68" s="45" t="n"/>
+    </row>
+    <row r="69">
+      <c r="B69" s="45" t="n"/>
+      <c r="C69" s="45" t="n"/>
+    </row>
+    <row r="70">
+      <c r="B70" s="45" t="n"/>
+      <c r="C70" s="45" t="n"/>
+    </row>
+    <row r="71">
+      <c r="B71" s="45" t="n"/>
+      <c r="C71" s="45" t="n"/>
+    </row>
+    <row r="72">
+      <c r="B72" s="45" t="n"/>
+      <c r="C72" s="45" t="n"/>
+    </row>
+    <row r="73">
+      <c r="B73" s="45" t="n"/>
+      <c r="C73" s="45" t="n"/>
+    </row>
+    <row r="74">
+      <c r="B74" s="45" t="n"/>
+      <c r="C74" s="45" t="n"/>
+    </row>
+    <row r="75">
+      <c r="B75" s="45" t="n"/>
+      <c r="C75" s="45" t="n"/>
+    </row>
+    <row r="76">
+      <c r="B76" s="45" t="n"/>
+      <c r="C76" s="45" t="n"/>
+    </row>
+    <row r="77">
+      <c r="B77" s="45" t="n"/>
+      <c r="C77" s="45" t="n"/>
+    </row>
+    <row r="78">
+      <c r="B78" s="45" t="n"/>
+      <c r="C78" s="45" t="n"/>
+    </row>
+    <row r="79">
+      <c r="B79" s="45" t="n"/>
+      <c r="C79" s="45" t="n"/>
+    </row>
+    <row r="80">
+      <c r="B80" s="45" t="n"/>
+      <c r="C80" s="45" t="n"/>
+    </row>
+    <row r="81">
+      <c r="B81" s="45" t="n"/>
+      <c r="C81" s="45" t="n"/>
+    </row>
+    <row r="82">
+      <c r="B82" s="45" t="n"/>
+      <c r="C82" s="45" t="n"/>
+    </row>
+    <row r="83">
+      <c r="B83" s="45" t="n"/>
+      <c r="C83" s="45" t="n"/>
+    </row>
+    <row r="84">
+      <c r="B84" s="45" t="n"/>
+      <c r="C84" s="45" t="n"/>
+    </row>
+    <row r="85">
+      <c r="B85" s="45" t="n"/>
+      <c r="C85" s="45" t="n"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="45" t="n"/>
+      <c r="C86" s="45" t="n"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="45" t="n"/>
+      <c r="C87" s="45" t="n"/>
+    </row>
+    <row r="88">
+      <c r="B88" s="45" t="n"/>
+      <c r="C88" s="45" t="n"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="45" t="n"/>
+      <c r="C89" s="45" t="n"/>
+    </row>
+    <row r="90">
+      <c r="B90" s="45" t="n"/>
+      <c r="C90" s="45" t="n"/>
+    </row>
+    <row r="91">
+      <c r="B91" s="45" t="n"/>
+      <c r="C91" s="45" t="n"/>
+    </row>
+    <row r="92">
+      <c r="B92" s="45" t="n"/>
+      <c r="C92" s="45" t="n"/>
+    </row>
+    <row r="93">
+      <c r="B93" s="45" t="n"/>
+      <c r="C93" s="45" t="n"/>
+    </row>
+    <row r="94">
+      <c r="B94" s="45" t="n"/>
+      <c r="C94" s="45" t="n"/>
+    </row>
+    <row r="95">
+      <c r="B95" s="45" t="n"/>
+      <c r="C95" s="45" t="n"/>
+    </row>
+    <row r="96">
+      <c r="B96" s="45" t="n"/>
+      <c r="C96" s="45" t="n"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="45" t="n"/>
+      <c r="C97" s="45" t="n"/>
+    </row>
+    <row r="98">
+      <c r="B98" s="45" t="n"/>
+      <c r="C98" s="45" t="n"/>
+    </row>
+    <row r="99">
+      <c r="B99" s="45" t="n"/>
+      <c r="C99" s="45" t="n"/>
+    </row>
+    <row r="100">
+      <c r="B100" s="45" t="n"/>
+      <c r="C100" s="45" t="n"/>
+    </row>
+    <row r="101">
+      <c r="B101" s="45" t="n"/>
+      <c r="C101" s="45" t="n"/>
+    </row>
+    <row r="102">
+      <c r="B102" s="45" t="n"/>
+      <c r="C102" s="45" t="n"/>
+    </row>
+    <row r="103">
+      <c r="B103" s="45" t="n"/>
+      <c r="C103" s="45" t="n"/>
+    </row>
+    <row r="104">
+      <c r="B104" s="45" t="n"/>
+      <c r="C104" s="45" t="n"/>
+    </row>
+    <row r="105">
+      <c r="B105" s="45" t="n"/>
+      <c r="C105" s="45" t="n"/>
+    </row>
+    <row r="106">
+      <c r="B106" s="45" t="n"/>
+      <c r="C106" s="45" t="n"/>
+    </row>
+    <row r="107">
+      <c r="B107" s="45" t="n"/>
+      <c r="C107" s="45" t="n"/>
+    </row>
+    <row r="108">
+      <c r="B108" s="45" t="n"/>
+      <c r="C108" s="45" t="n"/>
+    </row>
+    <row r="109">
+      <c r="B109" s="45" t="n"/>
+      <c r="C109" s="45" t="n"/>
+    </row>
+    <row r="110">
+      <c r="B110" s="45" t="n"/>
+      <c r="C110" s="45" t="n"/>
+    </row>
+    <row r="111">
+      <c r="B111" s="45" t="n"/>
+      <c r="C111" s="45" t="n"/>
+    </row>
+    <row r="112">
+      <c r="B112" s="45" t="n"/>
+      <c r="C112" s="45" t="n"/>
+    </row>
+    <row r="113">
+      <c r="B113" s="45" t="n"/>
+      <c r="C113" s="45" t="n"/>
+    </row>
+    <row r="114">
+      <c r="B114" s="45" t="n"/>
+      <c r="C114" s="45" t="n"/>
+    </row>
+    <row r="115">
+      <c r="B115" s="45" t="n"/>
+      <c r="C115" s="45" t="n"/>
+    </row>
+    <row r="116">
+      <c r="B116" s="45" t="n"/>
+      <c r="C116" s="45" t="n"/>
+    </row>
+    <row r="117">
+      <c r="B117" s="45" t="n"/>
+      <c r="C117" s="45" t="n"/>
+    </row>
+    <row r="118">
+      <c r="B118" s="45" t="n"/>
+      <c r="C118" s="45" t="n"/>
+    </row>
+    <row r="119">
+      <c r="B119" s="45" t="n"/>
+      <c r="C119" s="45" t="n"/>
+    </row>
+    <row r="120">
+      <c r="B120" s="45" t="n"/>
+      <c r="C120" s="45" t="n"/>
+    </row>
+    <row r="121">
+      <c r="B121" s="45" t="n"/>
+      <c r="C121" s="45" t="n"/>
+    </row>
+    <row r="122">
+      <c r="B122" s="45" t="n"/>
+      <c r="C122" s="45" t="n"/>
+    </row>
+    <row r="123">
+      <c r="B123" s="45" t="n"/>
+      <c r="C123" s="45" t="n"/>
+    </row>
+    <row r="124">
+      <c r="B124" s="45" t="n"/>
+      <c r="C124" s="45" t="n"/>
+    </row>
+    <row r="125">
+      <c r="B125" s="45" t="n"/>
+      <c r="C125" s="45" t="n"/>
+    </row>
+    <row r="126">
+      <c r="B126" s="45" t="n"/>
+      <c r="C126" s="45" t="n"/>
+    </row>
+    <row r="127">
+      <c r="B127" s="45" t="n"/>
+      <c r="C127" s="45" t="n"/>
+    </row>
+    <row r="128">
+      <c r="B128" s="45" t="n"/>
+      <c r="C128" s="45" t="n"/>
+    </row>
+    <row r="129">
+      <c r="B129" s="45" t="n"/>
+      <c r="C129" s="45" t="n"/>
+    </row>
+    <row r="130">
+      <c r="B130" s="45" t="n"/>
+      <c r="C130" s="45" t="n"/>
+    </row>
+    <row r="131">
+      <c r="B131" s="45" t="n"/>
+      <c r="C131" s="45" t="n"/>
+    </row>
+    <row r="132">
+      <c r="B132" s="45" t="n"/>
+      <c r="C132" s="45" t="n"/>
+    </row>
+    <row r="133">
+      <c r="B133" s="45" t="n"/>
+      <c r="C133" s="45" t="n"/>
+    </row>
+    <row r="134">
+      <c r="B134" s="45" t="n"/>
+      <c r="C134" s="45" t="n"/>
+    </row>
+    <row r="135">
+      <c r="B135" s="45" t="n"/>
+      <c r="C135" s="45" t="n"/>
+    </row>
+    <row r="136">
+      <c r="B136" s="45" t="n"/>
+      <c r="C136" s="45" t="n"/>
+    </row>
+    <row r="137">
+      <c r="B137" s="45" t="n"/>
+      <c r="C137" s="45" t="n"/>
+    </row>
+    <row r="138">
+      <c r="B138" s="45" t="n"/>
+      <c r="C138" s="45" t="n"/>
+    </row>
+    <row r="139">
+      <c r="B139" s="45" t="n"/>
+      <c r="C139" s="45" t="n"/>
+    </row>
+    <row r="140">
+      <c r="B140" s="45" t="n"/>
+      <c r="C140" s="45" t="n"/>
+    </row>
+    <row r="141">
+      <c r="B141" s="45" t="n"/>
+      <c r="C141" s="45" t="n"/>
+    </row>
+    <row r="142">
+      <c r="B142" s="45" t="n"/>
+      <c r="C142" s="45" t="n"/>
+    </row>
+    <row r="143">
+      <c r="B143" s="45" t="n"/>
+      <c r="C143" s="45" t="n"/>
+    </row>
+    <row r="144">
+      <c r="B144" s="45" t="n"/>
+      <c r="C144" s="45" t="n"/>
+    </row>
+    <row r="145">
+      <c r="B145" s="45" t="n"/>
+      <c r="C145" s="45" t="n"/>
+    </row>
+    <row r="146">
+      <c r="B146" s="45" t="n"/>
+      <c r="C146" s="45" t="n"/>
+    </row>
+    <row r="147">
+      <c r="B147" s="45" t="n"/>
+      <c r="C147" s="45" t="n"/>
+    </row>
+    <row r="148">
+      <c r="B148" s="45" t="n"/>
+      <c r="C148" s="45" t="n"/>
+    </row>
+    <row r="149">
+      <c r="B149" s="45" t="n"/>
+      <c r="C149" s="45" t="n"/>
+    </row>
+    <row r="150">
+      <c r="B150" s="45" t="n"/>
+      <c r="C150" s="45" t="n"/>
+    </row>
+    <row r="151">
+      <c r="B151" s="45" t="n"/>
+      <c r="C151" s="45" t="n"/>
+    </row>
+    <row r="152">
+      <c r="B152" s="45" t="n"/>
+      <c r="C152" s="45" t="n"/>
+    </row>
+    <row r="153">
+      <c r="B153" s="45" t="n"/>
+      <c r="C153" s="45" t="n"/>
+    </row>
+    <row r="154">
+      <c r="B154" s="45" t="n"/>
+      <c r="C154" s="45" t="n"/>
+    </row>
+    <row r="155">
+      <c r="B155" s="45" t="n"/>
+      <c r="C155" s="45" t="n"/>
+    </row>
+    <row r="156">
+      <c r="B156" s="45" t="n"/>
+      <c r="C156" s="45" t="n"/>
+    </row>
+    <row r="157">
+      <c r="B157" s="45" t="n"/>
+      <c r="C157" s="45" t="n"/>
+    </row>
+    <row r="158">
+      <c r="B158" s="45" t="n"/>
+      <c r="C158" s="45" t="n"/>
+    </row>
+    <row r="159">
+      <c r="B159" s="45" t="n"/>
+      <c r="C159" s="45" t="n"/>
+    </row>
+    <row r="160">
+      <c r="B160" s="45" t="n"/>
+      <c r="C160" s="45" t="n"/>
+    </row>
+    <row r="161">
+      <c r="B161" s="45" t="n"/>
+      <c r="C161" s="45" t="n"/>
+    </row>
+    <row r="162">
+      <c r="B162" s="45" t="n"/>
+      <c r="C162" s="45" t="n"/>
+    </row>
+    <row r="163">
+      <c r="B163" s="45" t="n"/>
+      <c r="C163" s="45" t="n"/>
+    </row>
+    <row r="164">
+      <c r="B164" s="45" t="n"/>
+      <c r="C164" s="45" t="n"/>
+    </row>
+    <row r="165">
+      <c r="B165" s="45" t="n"/>
+      <c r="C165" s="45" t="n"/>
+    </row>
+    <row r="166">
+      <c r="B166" s="45" t="n"/>
+      <c r="C166" s="45" t="n"/>
+    </row>
+    <row r="167">
+      <c r="B167" s="45" t="n"/>
+      <c r="C167" s="45" t="n"/>
+    </row>
+    <row r="168">
+      <c r="B168" s="45" t="n"/>
+      <c r="C168" s="45" t="n"/>
+    </row>
+    <row r="169">
+      <c r="B169" s="45" t="n"/>
+      <c r="C169" s="45" t="n"/>
+    </row>
+    <row r="170">
+      <c r="B170" s="45" t="n"/>
+      <c r="C170" s="45" t="n"/>
+    </row>
+    <row r="171">
+      <c r="B171" s="45" t="n"/>
+      <c r="C171" s="45" t="n"/>
+    </row>
+    <row r="172">
+      <c r="B172" s="45" t="n"/>
+      <c r="C172" s="45" t="n"/>
+    </row>
+    <row r="173">
+      <c r="B173" s="45" t="n"/>
+      <c r="C173" s="45" t="n"/>
+    </row>
+    <row r="174">
+      <c r="B174" s="45" t="n"/>
+      <c r="C174" s="45" t="n"/>
+    </row>
+    <row r="175">
+      <c r="B175" s="45" t="n"/>
+      <c r="C175" s="45" t="n"/>
+    </row>
+    <row r="176">
+      <c r="B176" s="45" t="n"/>
+      <c r="C176" s="45" t="n"/>
+    </row>
+    <row r="177">
+      <c r="B177" s="45" t="n"/>
+      <c r="C177" s="45" t="n"/>
+    </row>
+    <row r="178">
+      <c r="B178" s="45" t="n"/>
+      <c r="C178" s="45" t="n"/>
+    </row>
+    <row r="179">
+      <c r="B179" s="45" t="n"/>
+      <c r="C179" s="45" t="n"/>
+    </row>
+    <row r="180">
+      <c r="B180" s="45" t="n"/>
+      <c r="C180" s="45" t="n"/>
+    </row>
+    <row r="181">
+      <c r="B181" s="45" t="n"/>
+      <c r="C181" s="45" t="n"/>
+    </row>
+    <row r="182">
+      <c r="B182" s="45" t="n"/>
+      <c r="C182" s="45" t="n"/>
+    </row>
+    <row r="183">
+      <c r="B183" s="45" t="n"/>
+      <c r="C183" s="45" t="n"/>
+    </row>
+    <row r="184">
+      <c r="B184" s="45" t="n"/>
+      <c r="C184" s="45" t="n"/>
+    </row>
+    <row r="185">
+      <c r="B185" s="45" t="n"/>
+      <c r="C185" s="45" t="n"/>
+    </row>
+    <row r="186">
+      <c r="B186" s="45" t="n"/>
+      <c r="C186" s="45" t="n"/>
+    </row>
+    <row r="187">
+      <c r="B187" s="45" t="n"/>
+      <c r="C187" s="45" t="n"/>
+    </row>
+    <row r="188">
+      <c r="B188" s="45" t="n"/>
+      <c r="C188" s="45" t="n"/>
+    </row>
+    <row r="189">
+      <c r="B189" s="45" t="n"/>
+      <c r="C189" s="45" t="n"/>
+    </row>
+    <row r="190">
+      <c r="B190" s="45" t="n"/>
+      <c r="C190" s="45" t="n"/>
+    </row>
+    <row r="191">
+      <c r="B191" s="45" t="n"/>
+      <c r="C191" s="45" t="n"/>
+    </row>
+    <row r="192">
+      <c r="B192" s="45" t="n"/>
+      <c r="C192" s="45" t="n"/>
+    </row>
+    <row r="193">
+      <c r="B193" s="45" t="n"/>
+      <c r="C193" s="45" t="n"/>
+    </row>
+    <row r="194">
+      <c r="B194" s="45" t="n"/>
+      <c r="C194" s="45" t="n"/>
+    </row>
+    <row r="195">
+      <c r="B195" s="45" t="n"/>
+      <c r="C195" s="45" t="n"/>
+    </row>
+    <row r="196">
+      <c r="B196" s="45" t="n"/>
+      <c r="C196" s="45" t="n"/>
+    </row>
+    <row r="197">
+      <c r="B197" s="45" t="n"/>
+      <c r="C197" s="45" t="n"/>
+    </row>
+    <row r="198">
+      <c r="B198" s="45" t="n"/>
+      <c r="C198" s="45" t="n"/>
+    </row>
+    <row r="199">
+      <c r="B199" s="45" t="n"/>
+      <c r="C199" s="45" t="n"/>
+    </row>
+    <row r="200">
+      <c r="B200" s="45" t="n"/>
+      <c r="C200" s="45" t="n"/>
+    </row>
+    <row r="201">
+      <c r="B201" s="45" t="n"/>
+      <c r="C201" s="45" t="n"/>
+    </row>
+    <row r="202">
+      <c r="B202" s="45" t="n"/>
+      <c r="C202" s="45" t="n"/>
+    </row>
+    <row r="203">
+      <c r="B203" s="45" t="n"/>
+      <c r="C203" s="45" t="n"/>
+    </row>
+    <row r="204">
+      <c r="B204" s="45" t="n"/>
+      <c r="C204" s="45" t="n"/>
+    </row>
+    <row r="205">
+      <c r="B205" s="45" t="n"/>
+      <c r="C205" s="45" t="n"/>
+    </row>
+    <row r="206">
+      <c r="B206" s="45" t="n"/>
+      <c r="C206" s="45" t="n"/>
+    </row>
+    <row r="207">
+      <c r="B207" s="45" t="n"/>
+      <c r="C207" s="45" t="n"/>
+    </row>
+    <row r="208">
+      <c r="B208" s="45" t="n"/>
+      <c r="C208" s="45" t="n"/>
+    </row>
+    <row r="209">
+      <c r="B209" s="45" t="n"/>
+      <c r="C209" s="45" t="n"/>
+    </row>
+    <row r="210">
+      <c r="B210" s="45" t="n"/>
+      <c r="C210" s="45" t="n"/>
+    </row>
+    <row r="211">
+      <c r="B211" s="45" t="n"/>
+      <c r="C211" s="45" t="n"/>
+    </row>
+    <row r="212">
+      <c r="B212" s="45" t="n"/>
+      <c r="C212" s="45" t="n"/>
+    </row>
+    <row r="213">
+      <c r="B213" s="45" t="n"/>
+      <c r="C213" s="45" t="n"/>
+    </row>
+    <row r="214">
+      <c r="B214" s="45" t="n"/>
+      <c r="C214" s="45" t="n"/>
+    </row>
+    <row r="215">
+      <c r="B215" s="45" t="n"/>
+      <c r="C215" s="45" t="n"/>
+    </row>
+    <row r="216">
+      <c r="B216" s="45" t="n"/>
+      <c r="C216" s="45" t="n"/>
+    </row>
+    <row r="217">
+      <c r="B217" s="45" t="n"/>
+      <c r="C217" s="45" t="n"/>
+    </row>
+    <row r="218">
+      <c r="B218" s="45" t="n"/>
+      <c r="C218" s="45" t="n"/>
+    </row>
+    <row r="219">
+      <c r="B219" s="45" t="n"/>
+      <c r="C219" s="45" t="n"/>
+    </row>
+    <row r="220">
+      <c r="B220" s="45" t="n"/>
+      <c r="C220" s="45" t="n"/>
+    </row>
+    <row r="221">
+      <c r="B221" s="45" t="n"/>
+      <c r="C221" s="45" t="n"/>
+    </row>
+    <row r="222">
+      <c r="B222" s="45" t="n"/>
+      <c r="C222" s="45" t="n"/>
+    </row>
+    <row r="223">
+      <c r="B223" s="45" t="n"/>
+      <c r="C223" s="45" t="n"/>
+    </row>
+    <row r="224">
+      <c r="B224" s="45" t="n"/>
+      <c r="C224" s="45" t="n"/>
+    </row>
+    <row r="225">
+      <c r="B225" s="45" t="n"/>
+      <c r="C225" s="45" t="n"/>
+    </row>
+    <row r="226">
+      <c r="B226" s="45" t="n"/>
+      <c r="C226" s="45" t="n"/>
+    </row>
+    <row r="227">
+      <c r="B227" s="45" t="n"/>
+      <c r="C227" s="45" t="n"/>
+    </row>
+    <row r="228">
+      <c r="B228" s="45" t="n"/>
+      <c r="C228" s="45" t="n"/>
+    </row>
+    <row r="229">
+      <c r="B229" s="45" t="n"/>
+      <c r="C229" s="45" t="n"/>
+    </row>
+    <row r="230">
+      <c r="B230" s="45" t="n"/>
+      <c r="C230" s="45" t="n"/>
+    </row>
+    <row r="231">
+      <c r="B231" s="45" t="n"/>
+      <c r="C231" s="45" t="n"/>
+    </row>
+    <row r="232">
+      <c r="B232" s="45" t="n"/>
+      <c r="C232" s="45" t="n"/>
+    </row>
+    <row r="233">
+      <c r="B233" s="45" t="n"/>
+      <c r="C233" s="45" t="n"/>
+    </row>
+    <row r="234">
+      <c r="B234" s="45" t="n"/>
+      <c r="C234" s="45" t="n"/>
+    </row>
+    <row r="235">
+      <c r="B235" s="45" t="n"/>
+      <c r="C235" s="45" t="n"/>
+    </row>
+    <row r="236">
+      <c r="B236" s="45" t="n"/>
+      <c r="C236" s="45" t="n"/>
+    </row>
+    <row r="237">
+      <c r="B237" s="45" t="n"/>
+      <c r="C237" s="45" t="n"/>
+    </row>
+    <row r="238">
+      <c r="B238" s="45" t="n"/>
+      <c r="C238" s="45" t="n"/>
+    </row>
+    <row r="239">
+      <c r="B239" s="45" t="n"/>
+      <c r="C239" s="45" t="n"/>
+    </row>
+    <row r="240">
+      <c r="B240" s="45" t="n"/>
+      <c r="C240" s="45" t="n"/>
+    </row>
+    <row r="241">
+      <c r="B241" s="45" t="n"/>
+      <c r="C241" s="45" t="n"/>
+    </row>
+    <row r="242">
+      <c r="B242" s="45" t="n"/>
+      <c r="C242" s="45" t="n"/>
+    </row>
+    <row r="243">
+      <c r="B243" s="45" t="n"/>
+      <c r="C243" s="45" t="n"/>
+    </row>
+    <row r="244">
+      <c r="B244" s="45" t="n"/>
+      <c r="C244" s="45" t="n"/>
+    </row>
+    <row r="245">
+      <c r="B245" s="45" t="n"/>
+      <c r="C245" s="45" t="n"/>
+    </row>
+    <row r="246">
+      <c r="B246" s="45" t="n"/>
+      <c r="C246" s="45" t="n"/>
+    </row>
+    <row r="247">
+      <c r="B247" s="45" t="n"/>
+      <c r="C247" s="45" t="n"/>
+    </row>
+    <row r="248">
+      <c r="B248" s="45" t="n"/>
+      <c r="C248" s="45" t="n"/>
+    </row>
+    <row r="249">
+      <c r="B249" s="45" t="n"/>
+      <c r="C249" s="45" t="n"/>
+    </row>
+    <row r="250">
+      <c r="B250" s="45" t="n"/>
+      <c r="C250" s="45" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
+  <mergeCells count="48">
     <mergeCell ref="G21:H21"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G37:H38"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="G27:H27"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="C1:H3"/>
+    <mergeCell ref="E14:F14"/>
     <mergeCell ref="B30:H30"/>
     <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="C1:H3"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="G40:H40"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="B32:H32"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="A33:H34"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="D29:F29"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A33:H33"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G20:H20"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D42:E42"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="D15:E15"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="G22:H22"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>